<commit_message>
Updating info.xlsx and template.xlsx | Implementing multiple PM header info
</commit_message>
<xml_diff>
--- a/src/base/template.xlsx
+++ b/src/base/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonio.castro\Documents\Envio de Horas - Script\scriptsPlanilhas\base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonio.castro\Documents\Envio de Horas - Script\worksheetAutomationScript\src\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FF505-264D-43B9-BCD9-B217F1F54FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16C8B2-F681-4F31-BD7B-96E8942E3CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -38,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Período</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorraina Izac (17) 99234 4017 </t>
-  </si>
-  <si>
     <t>Recurso</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>COL</t>
-  </si>
-  <si>
     <t>Gerente de Projetos</t>
   </si>
   <si>
@@ -106,21 +100,12 @@
     <t>Responsáveis</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorraina Silva (17) 99234-4017            </t>
-  </si>
-  <si>
     <t xml:space="preserve">Centro de Custo Pagador </t>
   </si>
   <si>
-    <t>00001.00001.001.7.317</t>
-  </si>
-  <si>
     <t>Cood. TI Resposável</t>
   </si>
   <si>
-    <t>Reginaldo Nicola</t>
-  </si>
-  <si>
     <t>Consolidado por SQUAD</t>
   </si>
   <si>
@@ -131,6 +116,9 @@
   </si>
   <si>
     <t>Gerente de projetos</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -704,6 +692,21 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -749,21 +752,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="11" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1052,8 +1040,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1072,9 +1060,7 @@
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
-      <c r="D1" s="40" t="s">
-        <v>1</v>
-      </c>
+      <c r="D1" s="40"/>
       <c r="E1" s="40"/>
       <c r="F1" s="40"/>
       <c r="G1" s="2"/>
@@ -1102,7 +1088,7 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="41" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" s="41"/>
       <c r="F2" s="41"/>
@@ -1155,7 +1141,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="37"/>
@@ -1211,16 +1197,16 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="11"/>
@@ -1300,22 +1286,22 @@
     </row>
     <row r="9" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="C9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>12</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1896,7 +1882,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A3" sqref="A3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1905,153 +1891,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="44"/>
+      <c r="A1" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="49"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="54"/>
-      <c r="O2" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="54"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="59"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47">
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52">
         <v>0</v>
       </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="55" t="str">
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="60">
         <f>CABEÇALHO!B10</f>
-        <v>00001.00001.001.7.317</v>
-      </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56">
+        <v>0</v>
+      </c>
+      <c r="L3" s="60"/>
+      <c r="M3" s="61">
         <f>SUM(H3:H6)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="str">
+      <c r="N3" s="61"/>
+      <c r="O3" s="62">
         <f>CABEÇALHO!B12</f>
-        <v>Reginaldo Nicola</v>
-      </c>
-      <c r="P3" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="62"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="51">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="56">
         <v>0</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="51">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="56">
         <v>0</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="51">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="56">
         <v>0</v>
       </c>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="28"/>
@@ -2067,6 +2051,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="K3:L6"/>
+    <mergeCell ref="M3:N6"/>
+    <mergeCell ref="O3:P6"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:J2"/>
@@ -2083,9 +2070,6 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
-    <mergeCell ref="K3:L6"/>
-    <mergeCell ref="M3:N6"/>
-    <mergeCell ref="O3:P6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2100,20 +2084,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D34B99E-854E-4DA2-9CC8-C8BB4373F316}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="65"/>
@@ -2133,20 +2117,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="70"/>
-      <c r="B5" s="31">
-        <v>46012</v>
-      </c>
-      <c r="C5" s="31">
-        <v>46042</v>
-      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
@@ -2155,27 +2135,25 @@
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="72" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7" s="68"/>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="70"/>
       <c r="B8" s="73" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="68"/>
     </row>
     <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>24</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B10" s="33"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="34"/>
@@ -2183,11 +2161,9 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>26</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B12" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Implementing Excel formulas in columns B and E
</commit_message>
<xml_diff>
--- a/src/base/template.xlsx
+++ b/src/base/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonio.castro\Documents\Envio de Horas - Script\worksheetAutomationScript\src\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16C8B2-F681-4F31-BD7B-96E8942E3CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C96CD7-FDDA-44F7-838A-308C43326D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -330,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -423,17 +423,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalDown="1">
@@ -589,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -652,16 +641,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -692,40 +678,25 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -753,25 +724,40 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="11" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1038,10 +1024,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:Z1048356"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1055,14 +1041,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1084,14 +1070,14 @@
       <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="41" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1140,12 +1126,12 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="8"/>
       <c r="F4" s="5"/>
       <c r="G4" s="2"/>
@@ -1169,10 +1155,10 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="9"/>
       <c r="F5" s="5"/>
       <c r="G5" s="2"/>
@@ -1233,7 +1219,7 @@
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14">
-        <f>SUM(E10:E100)</f>
+        <f>SUM(E10:E150)</f>
         <v>0</v>
       </c>
       <c r="E7" s="5"/>
@@ -1326,10 +1312,16 @@
     </row>
     <row r="10" spans="1:26" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
+      <c r="B10" s="21" t="str">
+        <f>TEXT(A10, "dddd")</f>
+        <v>sábado</v>
+      </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="E10" s="22">
+        <f>IF(D10="SIM",C10*2,C10)</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
@@ -1352,9 +1344,7 @@
       <c r="Y10" s="24"/>
       <c r="Z10" s="24"/>
     </row>
-    <row r="11" spans="1:26" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-    </row>
+    <row r="11" spans="1:26" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:26" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:26" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:26" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1624,244 +1614,24 @@
     <row r="278" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="279" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="280" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048558" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048559" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048560" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048561" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048562" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048563" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048564" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048565" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048566" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048567" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048568" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048569" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048570" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048339" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048340" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048341" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048342" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048343" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048344" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048345" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048346" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048347" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048348" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048349" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048350" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048351" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048352" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048353" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048354" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048355" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048356" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A4:A5"/>
@@ -1887,173 +1657,170 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="11.5703125" style="27"/>
+    <col min="1" max="16384" width="11.5703125" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="49"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="58" t="s">
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58" t="s">
+      <c r="L2" s="52"/>
+      <c r="M2" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="59"/>
-      <c r="O2" s="58" t="s">
+      <c r="N2" s="53"/>
+      <c r="O2" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="59"/>
+      <c r="P2" s="53"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52">
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46">
         <v>0</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="60">
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="54">
         <f>CABEÇALHO!B10</f>
         <v>0</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61">
+      <c r="L3" s="54"/>
+      <c r="M3" s="55">
         <f>SUM(H3:H6)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="61"/>
-      <c r="O3" s="62">
+      <c r="N3" s="55"/>
+      <c r="O3" s="56">
         <f>CABEÇALHO!B12</f>
         <v>0</v>
       </c>
-      <c r="P3" s="62"/>
+      <c r="P3" s="56"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="55" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56">
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="50">
         <v>0</v>
       </c>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="57" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="56">
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="50">
         <v>0</v>
       </c>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="57" t="s">
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="56">
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="50">
         <v>0</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="61"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="K3:L6"/>
-    <mergeCell ref="M3:N6"/>
-    <mergeCell ref="O3:P6"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:J2"/>
@@ -2070,6 +1837,9 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
+    <mergeCell ref="K3:L6"/>
+    <mergeCell ref="M3:N6"/>
+    <mergeCell ref="O3:P6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2084,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D34B99E-854E-4DA2-9CC8-C8BB4373F316}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
@@ -2096,74 +1866,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="65"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="64"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="67"/>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="70"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="67"/>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="70"/>
-      <c r="B8" s="73" t="s">
+      <c r="A8" s="69"/>
+      <c r="B8" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="68"/>
+      <c r="C8" s="67"/>
     </row>
     <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="33"/>
+      <c r="B10" s="32"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>